<commit_message>
[V1.4.19] -> Matcher highest priority unique elemanlar ile yapıldı -> Diller verisi güncellendi. -> Update JavaDoc -> Cluster training kodu güncellendi,
</commit_message>
<xml_diff>
--- a/data/diller.xlsx
+++ b/data/diller.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
   <si>
     <t>name</t>
   </si>
@@ -152,9 +152,6 @@
     <t>İgbo Dili</t>
   </si>
   <si>
-    <t>history</t>
-  </si>
-  <si>
     <t>İngilizce</t>
   </si>
   <si>
@@ -324,9 +321,6 @@
   </si>
   <si>
     <t>Telugu Dili</t>
-  </si>
-  <si>
-    <t>check</t>
   </si>
   <si>
     <t>Türkçe</t>
@@ -675,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A111"/>
+  <dimension ref="A1:A109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1228,16 +1222,6 @@
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>110</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>